<commit_message>
add better formatted field data
</commit_message>
<xml_diff>
--- a/data/FIELD DATA EXAMPLE 2023 gerry and marianne villages.xlsx
+++ b/data/FIELD DATA EXAMPLE 2023 gerry and marianne villages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gryan/Documents/tki_work/vector_atlas/vector_atlas_training_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43BB1E21-9E03-E941-82DC-BD5BFE8F9C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D8755F-5E94-3644-8E39-24EA95505207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-9680" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{B285063E-78B3-6A42-87D3-3F8199852D79}"/>
+    <workbookView xWindow="-51200" yWindow="-9680" windowWidth="51200" windowHeight="28800" xr2:uid="{B285063E-78B3-6A42-87D3-3F8199852D79}"/>
   </bookViews>
   <sheets>
     <sheet name="vill_gerry" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t>Village Gerry</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>Collector: Nick</t>
   </si>
 </sst>
 </file>
@@ -486,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565669E2-59D9-E24A-895D-4F9C18F5EFEE}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A35" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,6 +507,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
       <c r="B2">
         <v>1.55</v>
       </c>
@@ -783,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E631BE6-D94D-954A-BF75-0B45B06C8922}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>